<commit_message>
fix sum response from import dssv
</commit_message>
<xml_diff>
--- a/student/upload/loi-nhap-lieu-ds-diem.xlsx
+++ b/student/upload/loi-nhap-lieu-ds-diem.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Mã sinh viên</t>
   </si>
@@ -44,7 +44,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>20242</t>
+    <t>20222</t>
   </si>
   <si>
     <t>8.91</t>
@@ -62,24 +62,24 @@
     <t>Mã sv không tồn tại</t>
   </si>
   <si>
+    <t>6655051</t>
+  </si>
+  <si>
+    <t>7.15</t>
+  </si>
+  <si>
+    <t>2.86</t>
+  </si>
+  <si>
+    <t>7.18</t>
+  </si>
+  <si>
+    <t>2.87</t>
+  </si>
+  <si>
     <t>Học kỳ không tồn tại</t>
   </si>
   <si>
-    <t>6655051</t>
-  </si>
-  <si>
-    <t>7.15</t>
-  </si>
-  <si>
-    <t>2.86</t>
-  </si>
-  <si>
-    <t>7.18</t>
-  </si>
-  <si>
-    <t>2.87</t>
-  </si>
-  <si>
     <t>6652385</t>
   </si>
   <si>
@@ -98,6 +98,9 @@
     <t>ĐTB10 không hợp lệ</t>
   </si>
   <si>
+    <t>Dữ liệu của hàng này đã tồn tại</t>
+  </si>
+  <si>
     <t>6655419</t>
   </si>
   <si>
@@ -119,9 +122,6 @@
     <t>6667532</t>
   </si>
   <si>
-    <t>20211</t>
-  </si>
-  <si>
     <t>9.19</t>
   </si>
   <si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>3.69</t>
-  </si>
-  <si>
-    <t>Dữ liệu của hàng này đã tồn tại</t>
   </si>
   <si>
     <t>6666130</t>
@@ -241,8 +238,8 @@
       <c r="A2" t="s" s="1">
         <v>15</v>
       </c>
-      <c r="B2" t="s" s="1">
-        <v>16</v>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -251,10 +248,10 @@
         <v>12</v>
       </c>
       <c r="E2" t="n">
-        <v>103.0</v>
+        <v>102.0</v>
       </c>
       <c r="F2" t="n">
-        <v>96.0</v>
+        <v>82.0</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -265,29 +262,29 @@
       <c r="I2"/>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="1">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s" s="1">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s" s="1">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>91.0</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>20</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
       </c>
       <c r="I3"/>
     </row>
@@ -295,8 +292,8 @@
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s" s="1">
-        <v>16</v>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
       <c r="C4" t="s" s="1">
         <v>27</v>
@@ -305,10 +302,10 @@
         <v>24</v>
       </c>
       <c r="E4" t="n">
-        <v>97.0</v>
+        <v>86.0</v>
       </c>
       <c r="F4" t="n">
-        <v>87.0</v>
+        <v>82.0</v>
       </c>
       <c r="G4" t="s">
         <v>25</v>
@@ -316,41 +313,45 @@
       <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="I4"/>
+      <c r="I4" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s" s="1">
+        <v>34</v>
+      </c>
+      <c r="E5" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s" s="1">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s" s="1">
-        <v>33</v>
-      </c>
-      <c r="E5" t="n">
-        <v>75.0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>81.0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>36</v>
@@ -359,10 +360,10 @@
         <v>37</v>
       </c>
       <c r="E6" t="n">
-        <v>89.0</v>
+        <v>106.0</v>
       </c>
       <c r="F6" t="n">
-        <v>85.0</v>
+        <v>76.0</v>
       </c>
       <c r="G6" t="s">
         <v>38</v>
@@ -371,35 +372,37 @@
         <v>39</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s" s="1">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>94.0</v>
+      </c>
+      <c r="G7" t="s">
         <v>43</v>
       </c>
-      <c r="E7" t="n">
-        <v>27.0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>53.0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>44</v>
-      </c>
       <c r="H7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7"/>
+        <v>42</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>